<commit_message>
Added HW solutions and additional comments. Also, changed BaseClass to Base test so we no longer have to worry about overwriting the main webDriver value. This also removed the duplication of setup and teardown mthod with each new page object we add. Only tests extends BaseTest and everything else extends CommonMethods.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OrangeHrmData.xlsx
+++ b/src/test/resources/testdata/OrangeHrmData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpmeloche/Development/eclipse/workspace/MavenExample2/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpmeloche/Development/eclipse/workspace/MavenExample/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07271535-5599-C54D-B4F5-3762F6236B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B27EA0-9023-4741-9787-82A351994BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15400" yWindow="2520" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{5A4ED39C-36DF-6D4C-87BB-DC45341D7331}"/>
   </bookViews>
@@ -66,10 +66,10 @@
     <t>John Smith</t>
   </si>
   <si>
-    <t>jsmith</t>
-  </si>
-  <si>
     <t>Enabled</t>
+  </si>
+  <si>
+    <t>jsmith2</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,10 +488,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>

</xml_diff>